<commit_message>
changed big2 airline order
</commit_message>
<xml_diff>
--- a/Big_scenario.xlsx
+++ b/Big_scenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramb\PycharmProjects\OperationGoed\OperationsMaarDanGoed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66846336-EFBF-4226-8B6F-5E8CBF5BE1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFE7170-3E4F-444E-BDF4-8D05BB53F558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{79B91F4B-CA5E-4A45-AD7D-E616F8CD4CDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{79B91F4B-CA5E-4A45-AD7D-E616F8CD4CDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Flights" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="165">
   <si>
     <t>Flight no.</t>
   </si>
@@ -529,6 +529,12 @@
   </si>
   <si>
     <t>15:15:00</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -923,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71DB94B-8C4B-48E9-923F-F1D60482C4C0}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1965,7 +1971,7 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>124</v>
@@ -1995,7 +2001,7 @@
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>125</v>
@@ -2025,7 +2031,7 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>125</v>
@@ -2055,7 +2061,7 @@
         <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>126</v>
@@ -2085,7 +2091,7 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>127</v>
@@ -2115,7 +2121,7 @@
         <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>127</v>
@@ -2145,7 +2151,7 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>128</v>
@@ -2175,7 +2181,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>129</v>
@@ -2205,7 +2211,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>130</v>
@@ -2235,7 +2241,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>130</v>
@@ -2265,7 +2271,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>131</v>
@@ -2295,7 +2301,7 @@
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>132</v>
@@ -2325,7 +2331,7 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>133</v>
@@ -2355,7 +2361,7 @@
         <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>134</v>
@@ -2385,7 +2391,7 @@
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>135</v>
@@ -2415,7 +2421,7 @@
         <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>135</v>
@@ -2445,7 +2451,7 @@
         <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>135</v>
@@ -2475,7 +2481,7 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>135</v>
@@ -2505,7 +2511,7 @@
         <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>136</v>
@@ -2535,7 +2541,7 @@
         <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>136</v>
@@ -2565,7 +2571,7 @@
         <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>137</v>
@@ -2595,7 +2601,7 @@
         <v>43</v>
       </c>
       <c r="C56" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>138</v>
@@ -2625,7 +2631,7 @@
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>139</v>
@@ -2655,7 +2661,7 @@
         <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>140</v>
@@ -2685,7 +2691,7 @@
         <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>141</v>

</xml_diff>